<commit_message>
updated g reviews cleaning
idk why my python file didn't save but here's the actual version
</commit_message>
<xml_diff>
--- a/data/google_reviews/google reviews cleaned df_no_text.xlsx
+++ b/data/google_reviews/google reviews cleaned df_no_text.xlsx
@@ -440,42 +440,42 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Stars</t>
+          <t>rating</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Reservation recommended</t>
+          <t>reservation_recommended</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Visited on</t>
+          <t>visited_on</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Wait time</t>
+          <t>wait_time</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Published date</t>
+          <t>published_date</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>isLocalGuide</t>
+          <t>is_local_guide</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Original language</t>
+          <t>original_language</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Cleaned Text</t>
+          <t>review_text</t>
         </is>
       </c>
     </row>

</xml_diff>